<commit_message>
Add maximal tax for dividends
</commit_message>
<xml_diff>
--- a/examples/Ucetni-kniha-Akcie.xlsx
+++ b/examples/Ucetni-kniha-Akcie.xlsx
@@ -1,86 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="BUY" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="SELL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="DIVIDEND" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ADDITIONAL FEE" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ADDITIONAL INCOME" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="BUY" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SELL" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DIVIDEND" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ADDITIONAL FEE" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ADDITIONAL INCOME" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BUY!$A$1:$J$999</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SELL!$A$1:$J$995</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">DIVIDEND!$A$1:$H$995</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ADDITIONAL FEE'!$A$1:$E$1000</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ADDITIONAL INCOME'!$A$1:$E$1000</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'ADDITIONAL FEE'!$A$1:$E$1000</definedName>
+    <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'ADDITIONAL INCOME'!$A$1:$E$1000</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">BUY!$A$1:$J$999</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">DIVIDEND!$A$1:$I$995</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">SELL!$A$1:$J$995</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
   <si>
-    <t>STOCK</t>
+    <t xml:space="preserve">STOCK</t>
   </si>
   <si>
-    <t>DATE</t>
+    <t xml:space="preserve">DATE</t>
   </si>
   <si>
     <t xml:space="preserve">STOCK PRICE</t>
   </si>
   <si>
-    <t>PAID</t>
+    <t xml:space="preserve">PAID</t>
   </si>
   <si>
-    <t>FEE</t>
+    <t xml:space="preserve">FEE</t>
   </si>
   <si>
-    <t>AMOUNT</t>
+    <t xml:space="preserve">AMOUNT</t>
   </si>
   <si>
-    <t>QUANTITY</t>
+    <t xml:space="preserve">QUANTITY</t>
   </si>
   <si>
-    <t>BROKER</t>
+    <t xml:space="preserve">BROKER</t>
   </si>
   <si>
-    <t>CURRENCY</t>
+    <t xml:space="preserve">CURRENCY</t>
   </si>
   <si>
-    <t>NOTES</t>
+    <t xml:space="preserve">NOTES</t>
   </si>
   <si>
-    <t>ABC</t>
+    <t xml:space="preserve">ABC</t>
   </si>
   <si>
-    <t>Revolut</t>
+    <t xml:space="preserve">Revolut</t>
   </si>
   <si>
-    <t>USD</t>
+    <t xml:space="preserve">USD</t>
   </si>
   <si>
-    <t>RECEIVED</t>
+    <t xml:space="preserve">RECEIVED</t>
   </si>
   <si>
     <t xml:space="preserve">PAID TAX</t>
   </si>
   <si>
-    <t>LOCATION</t>
+    <t xml:space="preserve">COUNTRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCATION</t>
   </si>
   <si>
     <t xml:space="preserve">Custody fee</t>
   </si>
   <si>
-    <t>EquatePlus</t>
+    <t xml:space="preserve">EquatePlus</t>
   </si>
   <si>
-    <t>EUR</t>
+    <t xml:space="preserve">EUR</t>
   </si>
   <si>
     <t xml:space="preserve">stock received as bonus</t>
@@ -89,28 +108,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
-    <numFmt numFmtId="160" formatCode="d&quot;.&quot;m&quot;.&quot;yyyy"/>
-    <numFmt numFmtId="161" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="162" formatCode="#,##0.00000000"/>
-    <numFmt numFmtId="163" formatCode="[$€]#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="[$$]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;&quot;$&quot;#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="10">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="d\.m\.yyyy"/>
+    <numFmt numFmtId="166" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="168" formatCode="[$€]#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0%"/>
+    <numFmt numFmtId="170" formatCode="0.00%"/>
+    <numFmt numFmtId="171" formatCode="[$$]#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="\$#,##0.00;\$#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color indexed="64"/>
-      <sz val="10.000000"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <color theme="1"/>
+      <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
-      <color indexed="64"/>
+      <family val="0"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +164,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -130,550 +172,151 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+  <cellXfs count="14">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="163" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="10" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="4" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
-  <a:themeElements>
-    <a:clrScheme name="Sheets">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4285F4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="EA4335"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="FBBC04"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="34A853"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="FF6D01"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="46BDC6"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="1155CC"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="1155CC"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Sheets">
-      <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-</a:theme>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:J190"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -705,28 +348,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
-        <v>43913.790856481479</v>
-      </c>
-      <c r="C2" s="3">
-        <v>357.49000000000001</v>
-      </c>
-      <c r="D2" s="3">
-        <f>F2+E2</f>
+      <c r="B2" s="2" t="n">
+        <v>43913.7908564815</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>357.49</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <f aca="false">F2+E2</f>
         <v>25</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="G2" s="4">
-        <v>0.069932019999999998</v>
+      <c r="G2" s="4" t="n">
+        <v>0.06993202</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -735,7 +378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -747,7 +390,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
@@ -759,7 +402,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
@@ -771,7 +414,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="3"/>
@@ -783,7 +426,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3"/>
@@ -795,7 +438,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -807,7 +450,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3"/>
@@ -819,7 +462,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
@@ -831,7 +474,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
@@ -843,7 +486,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
@@ -855,7 +498,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
@@ -867,7 +510,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
@@ -879,7 +522,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
@@ -891,7 +534,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="3"/>
@@ -903,7 +546,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
@@ -915,7 +558,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
@@ -927,7 +570,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="3"/>
@@ -939,7 +582,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
@@ -951,7 +594,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="3"/>
@@ -963,7 +606,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="3"/>
@@ -975,7 +618,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="3"/>
@@ -987,7 +630,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
@@ -999,7 +642,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
@@ -1011,7 +654,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="3"/>
@@ -1023,7 +666,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -1035,7 +678,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="3"/>
@@ -1047,7 +690,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="3"/>
@@ -1059,7 +702,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="3"/>
@@ -1071,7 +714,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="3"/>
@@ -1083,7 +726,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="3"/>
@@ -1095,7 +738,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
@@ -1107,7 +750,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="3"/>
@@ -1119,7 +762,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
@@ -1131,7 +774,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="3"/>
@@ -1143,7 +786,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="3"/>
@@ -1155,7 +798,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1"/>
       <c r="B38" s="5"/>
       <c r="C38" s="3"/>
@@ -1167,7 +810,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1"/>
       <c r="B39" s="5"/>
       <c r="C39" s="3"/>
@@ -1179,7 +822,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1"/>
       <c r="B40" s="5"/>
       <c r="C40" s="3"/>
@@ -1191,7 +834,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
       <c r="B41" s="5"/>
       <c r="C41" s="3"/>
@@ -1203,7 +846,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="5"/>
       <c r="C42" s="3"/>
@@ -1215,7 +858,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
       <c r="B43" s="5"/>
       <c r="C43" s="3"/>
@@ -1227,7 +870,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1"/>
       <c r="B44" s="5"/>
       <c r="C44" s="7"/>
@@ -1239,7 +882,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="5"/>
       <c r="C45" s="7"/>
@@ -1251,7 +894,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
       <c r="B46" s="5"/>
       <c r="C46" s="7"/>
@@ -1263,7 +906,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
       <c r="B47" s="5"/>
       <c r="C47" s="7"/>
@@ -1275,7 +918,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
       <c r="B48" s="5"/>
       <c r="C48" s="7"/>
@@ -1287,7 +930,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
       <c r="B49" s="5"/>
       <c r="C49" s="7"/>
@@ -1299,7 +942,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
       <c r="B50" s="5"/>
       <c r="C50" s="7"/>
@@ -1311,7 +954,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
       <c r="B51" s="5"/>
       <c r="C51" s="7"/>
@@ -1323,7 +966,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="5"/>
       <c r="C52" s="7"/>
@@ -1335,7 +978,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="B53" s="5"/>
       <c r="C53" s="7"/>
@@ -1347,7 +990,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="B54" s="5"/>
       <c r="C54" s="7"/>
@@ -1359,7 +1002,7 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
       <c r="B55" s="5"/>
       <c r="C55" s="7"/>
@@ -1371,7 +1014,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
       <c r="B56" s="5"/>
       <c r="C56" s="7"/>
@@ -1383,7 +1026,7 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
       <c r="B57" s="5"/>
       <c r="C57" s="7"/>
@@ -1395,7 +1038,7 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
       <c r="B58" s="5"/>
       <c r="C58" s="7"/>
@@ -1407,7 +1050,7 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1"/>
       <c r="B59" s="5"/>
       <c r="C59" s="7"/>
@@ -1419,7 +1062,7 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
       <c r="B60" s="5"/>
       <c r="C60" s="7"/>
@@ -1431,7 +1074,7 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
       <c r="B61" s="5"/>
       <c r="C61" s="7"/>
@@ -1443,7 +1086,7 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
       <c r="B62" s="5"/>
       <c r="C62" s="7"/>
@@ -1455,7 +1098,7 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
       <c r="B63" s="5"/>
       <c r="C63" s="7"/>
@@ -1467,7 +1110,7 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1"/>
       <c r="B64" s="5"/>
       <c r="C64" s="7"/>
@@ -1479,7 +1122,7 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1"/>
       <c r="B65" s="5"/>
       <c r="C65" s="7"/>
@@ -1491,7 +1134,7 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66">
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1"/>
       <c r="B66" s="5"/>
       <c r="C66" s="7"/>
@@ -1503,7 +1146,7 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67">
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1"/>
       <c r="B67" s="5"/>
       <c r="C67" s="7"/>
@@ -1515,7 +1158,7 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68">
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
       <c r="B68" s="5"/>
       <c r="C68" s="7"/>
@@ -1527,7 +1170,7 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69">
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
       <c r="B69" s="5"/>
       <c r="C69" s="7"/>
@@ -1539,7 +1182,7 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70">
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="B70" s="5"/>
       <c r="C70" s="7"/>
@@ -1551,7 +1194,7 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71">
+    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
       <c r="B71" s="5"/>
       <c r="C71" s="7"/>
@@ -1563,7 +1206,7 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72">
+    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1"/>
       <c r="B72" s="5"/>
       <c r="C72" s="7"/>
@@ -1575,7 +1218,7 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73">
+    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
       <c r="B73" s="5"/>
       <c r="C73" s="7"/>
@@ -1587,7 +1230,7 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74">
+    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1"/>
       <c r="B74" s="5"/>
       <c r="C74" s="7"/>
@@ -1599,7 +1242,7 @@
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75">
+    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
       <c r="B75" s="5"/>
       <c r="C75" s="7"/>
@@ -1611,7 +1254,7 @@
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76">
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1"/>
       <c r="B76" s="5"/>
       <c r="C76" s="7"/>
@@ -1623,7 +1266,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77">
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1"/>
       <c r="B77" s="5"/>
       <c r="C77" s="7"/>
@@ -1635,7 +1278,7 @@
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78">
+    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1"/>
       <c r="B78" s="5"/>
       <c r="C78" s="7"/>
@@ -1647,7 +1290,7 @@
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79">
+    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1"/>
       <c r="B79" s="5"/>
       <c r="C79" s="7"/>
@@ -1659,7 +1302,7 @@
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80">
+    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
       <c r="B80" s="5"/>
       <c r="C80" s="7"/>
@@ -1671,7 +1314,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81">
+    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
       <c r="B81" s="5"/>
       <c r="C81" s="7"/>
@@ -1683,7 +1326,7 @@
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82">
+    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
       <c r="B82" s="5"/>
       <c r="C82" s="7"/>
@@ -1695,7 +1338,7 @@
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83">
+    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1"/>
       <c r="B83" s="5"/>
       <c r="C83" s="7"/>
@@ -1707,7 +1350,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84">
+    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1"/>
       <c r="B84" s="5"/>
       <c r="C84" s="7"/>
@@ -1719,7 +1362,7 @@
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85">
+    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
       <c r="B85" s="5"/>
       <c r="C85" s="7"/>
@@ -1731,7 +1374,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86">
+    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
       <c r="B86" s="5"/>
       <c r="C86" s="7"/>
@@ -1743,7 +1386,7 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87">
+    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1"/>
       <c r="B87" s="5"/>
       <c r="C87" s="7"/>
@@ -1755,7 +1398,7 @@
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88">
+    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
       <c r="B88" s="5"/>
       <c r="C88" s="7"/>
@@ -1767,7 +1410,7 @@
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89">
+    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1"/>
       <c r="B89" s="5"/>
       <c r="C89" s="7"/>
@@ -1779,7 +1422,7 @@
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90">
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
       <c r="B90" s="5"/>
       <c r="C90" s="7"/>
@@ -1791,7 +1434,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91">
+    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1"/>
       <c r="B91" s="5"/>
       <c r="C91" s="7"/>
@@ -1803,7 +1446,7 @@
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92">
+    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1"/>
       <c r="B92" s="5"/>
       <c r="C92" s="7"/>
@@ -1815,7 +1458,7 @@
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93">
+    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1"/>
       <c r="B93" s="5"/>
       <c r="C93" s="7"/>
@@ -1827,7 +1470,7 @@
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94">
+    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1"/>
       <c r="B94" s="5"/>
       <c r="C94" s="7"/>
@@ -1839,7 +1482,7 @@
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95">
+    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
       <c r="B95" s="5"/>
       <c r="C95" s="7"/>
@@ -1851,7 +1494,7 @@
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96">
+    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1"/>
       <c r="B96" s="5"/>
       <c r="C96" s="7"/>
@@ -1863,7 +1506,7 @@
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97">
+    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
       <c r="B97" s="5"/>
       <c r="C97" s="7"/>
@@ -1875,7 +1518,7 @@
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98">
+    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
       <c r="B98" s="5"/>
       <c r="C98" s="7"/>
@@ -1887,7 +1530,7 @@
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99">
+    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1"/>
       <c r="B99" s="5"/>
       <c r="C99" s="7"/>
@@ -1899,7 +1542,7 @@
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100">
+    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
       <c r="B100" s="5"/>
       <c r="C100" s="7"/>
@@ -1911,7 +1554,7 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101">
+    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1"/>
       <c r="B101" s="5"/>
       <c r="C101" s="7"/>
@@ -1923,7 +1566,7 @@
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102">
+    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1"/>
       <c r="B102" s="5"/>
       <c r="C102" s="7"/>
@@ -1935,7 +1578,7 @@
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103">
+    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1"/>
       <c r="B103" s="5"/>
       <c r="C103" s="7"/>
@@ -1947,7 +1590,7 @@
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104">
+    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1"/>
       <c r="B104" s="5"/>
       <c r="C104" s="7"/>
@@ -1959,7 +1602,7 @@
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105">
+    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
       <c r="B105" s="5"/>
       <c r="C105" s="7"/>
@@ -1971,7 +1614,7 @@
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106">
+    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
       <c r="B106" s="5"/>
       <c r="C106" s="7"/>
@@ -1983,7 +1626,7 @@
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107">
+    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
       <c r="B107" s="5"/>
       <c r="C107" s="7"/>
@@ -1995,7 +1638,7 @@
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108">
+    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
       <c r="B108" s="5"/>
       <c r="C108" s="7"/>
@@ -2007,7 +1650,7 @@
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109">
+    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
       <c r="B109" s="5"/>
       <c r="C109" s="7"/>
@@ -2019,7 +1662,7 @@
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110">
+    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="B110" s="5"/>
       <c r="C110" s="7"/>
@@ -2031,7 +1674,7 @@
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
     </row>
-    <row r="111">
+    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="B111" s="5"/>
       <c r="C111" s="7"/>
@@ -2043,7 +1686,7 @@
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
-    <row r="112">
+    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
       <c r="B112" s="5"/>
       <c r="C112" s="7"/>
@@ -2055,7 +1698,7 @@
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
     </row>
-    <row r="113">
+    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1"/>
       <c r="B113" s="5"/>
       <c r="C113" s="7"/>
@@ -2067,7 +1710,7 @@
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114">
+    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="B114" s="5"/>
       <c r="C114" s="7"/>
@@ -2079,7 +1722,7 @@
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115">
+    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="B115" s="5"/>
       <c r="C115" s="7"/>
@@ -2091,7 +1734,7 @@
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116">
+    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="B116" s="5"/>
       <c r="C116" s="7"/>
@@ -2103,7 +1746,7 @@
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
-    <row r="117">
+    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
       <c r="B117" s="5"/>
       <c r="C117" s="7"/>
@@ -2115,7 +1758,7 @@
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
-    <row r="118">
+    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1"/>
       <c r="B118" s="5"/>
       <c r="C118" s="7"/>
@@ -2127,7 +1770,7 @@
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119">
+    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
       <c r="B119" s="5"/>
       <c r="C119" s="7"/>
@@ -2139,7 +1782,7 @@
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
-    <row r="120">
+    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="5"/>
       <c r="C120" s="7"/>
@@ -2151,7 +1794,7 @@
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
-    <row r="121">
+    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
       <c r="B121" s="5"/>
       <c r="C121" s="7"/>
@@ -2163,7 +1806,7 @@
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
     </row>
-    <row r="122">
+    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="5"/>
       <c r="C122" s="7"/>
@@ -2175,7 +1818,7 @@
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
     </row>
-    <row r="123">
+    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="5"/>
       <c r="C123" s="7"/>
@@ -2187,7 +1830,7 @@
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
-    <row r="124">
+    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1"/>
       <c r="B124" s="5"/>
       <c r="C124" s="7"/>
@@ -2199,7 +1842,7 @@
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
-    <row r="125">
+    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1"/>
       <c r="B125" s="5"/>
       <c r="C125" s="7"/>
@@ -2211,7 +1854,7 @@
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
-    <row r="126">
+    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
       <c r="B126" s="5"/>
       <c r="C126" s="7"/>
@@ -2223,7 +1866,7 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127">
+    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1"/>
       <c r="B127" s="5"/>
       <c r="C127" s="7"/>
@@ -2235,7 +1878,7 @@
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
-    <row r="128">
+    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
       <c r="B128" s="5"/>
       <c r="C128" s="7"/>
@@ -2247,7 +1890,7 @@
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
     </row>
-    <row r="129">
+    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
       <c r="B129" s="5"/>
       <c r="C129" s="7"/>
@@ -2259,7 +1902,7 @@
       <c r="I129" s="1"/>
       <c r="J129" s="1"/>
     </row>
-    <row r="130">
+    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
       <c r="B130" s="5"/>
       <c r="C130" s="7"/>
@@ -2271,7 +1914,7 @@
       <c r="I130" s="1"/>
       <c r="J130" s="1"/>
     </row>
-    <row r="131">
+    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
       <c r="B131" s="5"/>
       <c r="C131" s="7"/>
@@ -2283,7 +1926,7 @@
       <c r="I131" s="1"/>
       <c r="J131" s="1"/>
     </row>
-    <row r="132">
+    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1"/>
       <c r="B132" s="5"/>
       <c r="C132" s="7"/>
@@ -2295,7 +1938,7 @@
       <c r="I132" s="1"/>
       <c r="J132" s="1"/>
     </row>
-    <row r="133">
+    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1"/>
       <c r="B133" s="5"/>
       <c r="C133" s="7"/>
@@ -2307,7 +1950,7 @@
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
     </row>
-    <row r="134">
+    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
       <c r="B134" s="5"/>
       <c r="C134" s="7"/>
@@ -2319,7 +1962,7 @@
       <c r="I134" s="1"/>
       <c r="J134" s="1"/>
     </row>
-    <row r="135">
+    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
       <c r="B135" s="5"/>
       <c r="C135" s="7"/>
@@ -2331,7 +1974,7 @@
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
     </row>
-    <row r="136">
+    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
       <c r="B136" s="5"/>
       <c r="C136" s="7"/>
@@ -2343,7 +1986,7 @@
       <c r="I136" s="1"/>
       <c r="J136" s="1"/>
     </row>
-    <row r="137">
+    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
       <c r="B137" s="5"/>
       <c r="C137" s="7"/>
@@ -2355,7 +1998,7 @@
       <c r="I137" s="1"/>
       <c r="J137" s="1"/>
     </row>
-    <row r="138">
+    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
       <c r="B138" s="5"/>
       <c r="C138" s="7"/>
@@ -2367,7 +2010,7 @@
       <c r="I138" s="1"/>
       <c r="J138" s="1"/>
     </row>
-    <row r="139">
+    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
       <c r="B139" s="5"/>
       <c r="C139" s="7"/>
@@ -2379,7 +2022,7 @@
       <c r="I139" s="1"/>
       <c r="J139" s="1"/>
     </row>
-    <row r="140">
+    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1"/>
       <c r="B140" s="5"/>
       <c r="C140" s="7"/>
@@ -2391,7 +2034,7 @@
       <c r="I140" s="1"/>
       <c r="J140" s="1"/>
     </row>
-    <row r="141">
+    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
       <c r="B141" s="5"/>
       <c r="C141" s="7"/>
@@ -2403,7 +2046,7 @@
       <c r="I141" s="1"/>
       <c r="J141" s="1"/>
     </row>
-    <row r="142">
+    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
       <c r="B142" s="5"/>
       <c r="C142" s="7"/>
@@ -2415,7 +2058,7 @@
       <c r="I142" s="1"/>
       <c r="J142" s="1"/>
     </row>
-    <row r="143">
+    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
       <c r="B143" s="5"/>
       <c r="C143" s="7"/>
@@ -2427,7 +2070,7 @@
       <c r="I143" s="1"/>
       <c r="J143" s="1"/>
     </row>
-    <row r="144">
+    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
       <c r="B144" s="5"/>
       <c r="C144" s="7"/>
@@ -2439,7 +2082,7 @@
       <c r="I144" s="1"/>
       <c r="J144" s="1"/>
     </row>
-    <row r="145">
+    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
       <c r="B145" s="5"/>
       <c r="C145" s="7"/>
@@ -2451,7 +2094,7 @@
       <c r="I145" s="1"/>
       <c r="J145" s="1"/>
     </row>
-    <row r="146">
+    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1"/>
       <c r="B146" s="5"/>
       <c r="C146" s="7"/>
@@ -2463,7 +2106,7 @@
       <c r="I146" s="1"/>
       <c r="J146" s="1"/>
     </row>
-    <row r="147">
+    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
       <c r="B147" s="5"/>
       <c r="C147" s="7"/>
@@ -2475,7 +2118,7 @@
       <c r="I147" s="1"/>
       <c r="J147" s="1"/>
     </row>
-    <row r="148">
+    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
       <c r="B148" s="5"/>
       <c r="C148" s="7"/>
@@ -2487,7 +2130,7 @@
       <c r="I148" s="1"/>
       <c r="J148" s="1"/>
     </row>
-    <row r="149">
+    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
       <c r="B149" s="5"/>
       <c r="C149" s="7"/>
@@ -2499,7 +2142,7 @@
       <c r="I149" s="1"/>
       <c r="J149" s="1"/>
     </row>
-    <row r="150">
+    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
       <c r="B150" s="5"/>
       <c r="C150" s="7"/>
@@ -2511,7 +2154,7 @@
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
     </row>
-    <row r="151">
+    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
       <c r="B151" s="5"/>
       <c r="C151" s="7"/>
@@ -2523,7 +2166,7 @@
       <c r="I151" s="1"/>
       <c r="J151" s="1"/>
     </row>
-    <row r="152">
+    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
       <c r="B152" s="5"/>
       <c r="C152" s="7"/>
@@ -2535,7 +2178,7 @@
       <c r="I152" s="1"/>
       <c r="J152" s="1"/>
     </row>
-    <row r="153">
+    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1"/>
       <c r="B153" s="5"/>
       <c r="C153" s="7"/>
@@ -2547,7 +2190,7 @@
       <c r="I153" s="1"/>
       <c r="J153" s="1"/>
     </row>
-    <row r="154">
+    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
       <c r="B154" s="5"/>
       <c r="C154" s="7"/>
@@ -2559,7 +2202,7 @@
       <c r="I154" s="1"/>
       <c r="J154" s="1"/>
     </row>
-    <row r="155">
+    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
       <c r="B155" s="5"/>
       <c r="C155" s="7"/>
@@ -2571,7 +2214,7 @@
       <c r="I155" s="1"/>
       <c r="J155" s="1"/>
     </row>
-    <row r="156">
+    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
       <c r="B156" s="5"/>
       <c r="C156" s="7"/>
@@ -2583,7 +2226,7 @@
       <c r="I156" s="1"/>
       <c r="J156" s="1"/>
     </row>
-    <row r="157">
+    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
       <c r="B157" s="5"/>
       <c r="C157" s="7"/>
@@ -2595,7 +2238,7 @@
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
     </row>
-    <row r="158">
+    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
       <c r="B158" s="5"/>
       <c r="C158" s="7"/>
@@ -2607,7 +2250,7 @@
       <c r="I158" s="1"/>
       <c r="J158" s="1"/>
     </row>
-    <row r="159">
+    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
       <c r="B159" s="5"/>
       <c r="C159" s="7"/>
@@ -2619,7 +2262,7 @@
       <c r="I159" s="1"/>
       <c r="J159" s="1"/>
     </row>
-    <row r="160">
+    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
       <c r="B160" s="5"/>
       <c r="C160" s="7"/>
@@ -2631,7 +2274,7 @@
       <c r="I160" s="1"/>
       <c r="J160" s="1"/>
     </row>
-    <row r="161">
+    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1"/>
       <c r="B161" s="5"/>
       <c r="C161" s="7"/>
@@ -2643,7 +2286,7 @@
       <c r="I161" s="1"/>
       <c r="J161" s="1"/>
     </row>
-    <row r="162">
+    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="B162" s="5"/>
       <c r="C162" s="7"/>
@@ -2655,7 +2298,7 @@
       <c r="I162" s="1"/>
       <c r="J162" s="1"/>
     </row>
-    <row r="163">
+    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1"/>
       <c r="B163" s="5"/>
       <c r="C163" s="7"/>
@@ -2667,7 +2310,7 @@
       <c r="I163" s="1"/>
       <c r="J163" s="1"/>
     </row>
-    <row r="164">
+    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
       <c r="B164" s="5"/>
       <c r="C164" s="7"/>
@@ -2679,7 +2322,7 @@
       <c r="I164" s="1"/>
       <c r="J164" s="1"/>
     </row>
-    <row r="165">
+    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
       <c r="B165" s="5"/>
       <c r="C165" s="7"/>
@@ -2691,7 +2334,7 @@
       <c r="I165" s="1"/>
       <c r="J165" s="1"/>
     </row>
-    <row r="166">
+    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
       <c r="B166" s="5"/>
       <c r="C166" s="7"/>
@@ -2703,7 +2346,7 @@
       <c r="I166" s="1"/>
       <c r="J166" s="1"/>
     </row>
-    <row r="167">
+    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
       <c r="B167" s="5"/>
       <c r="C167" s="7"/>
@@ -2715,7 +2358,7 @@
       <c r="I167" s="1"/>
       <c r="J167" s="1"/>
     </row>
-    <row r="168">
+    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="5"/>
       <c r="C168" s="7"/>
@@ -2727,7 +2370,7 @@
       <c r="I168" s="1"/>
       <c r="J168" s="1"/>
     </row>
-    <row r="169">
+    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
       <c r="B169" s="5"/>
       <c r="C169" s="7"/>
@@ -2739,7 +2382,7 @@
       <c r="I169" s="1"/>
       <c r="J169" s="1"/>
     </row>
-    <row r="170">
+    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
       <c r="B170" s="5"/>
       <c r="C170" s="7"/>
@@ -2751,7 +2394,7 @@
       <c r="I170" s="1"/>
       <c r="J170" s="1"/>
     </row>
-    <row r="171">
+    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
       <c r="B171" s="5"/>
       <c r="C171" s="7"/>
@@ -2763,7 +2406,7 @@
       <c r="I171" s="1"/>
       <c r="J171" s="1"/>
     </row>
-    <row r="172">
+    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1"/>
       <c r="B172" s="5"/>
       <c r="C172" s="7"/>
@@ -2775,7 +2418,7 @@
       <c r="I172" s="1"/>
       <c r="J172" s="1"/>
     </row>
-    <row r="173">
+    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1"/>
       <c r="B173" s="5"/>
       <c r="C173" s="7"/>
@@ -2787,7 +2430,7 @@
       <c r="I173" s="1"/>
       <c r="J173" s="1"/>
     </row>
-    <row r="174">
+    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1"/>
       <c r="B174" s="5"/>
       <c r="C174" s="7"/>
@@ -2799,7 +2442,7 @@
       <c r="I174" s="1"/>
       <c r="J174" s="1"/>
     </row>
-    <row r="175">
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1"/>
       <c r="B175" s="5"/>
       <c r="C175" s="7"/>
@@ -2811,7 +2454,7 @@
       <c r="I175" s="1"/>
       <c r="J175" s="1"/>
     </row>
-    <row r="176">
+    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1"/>
       <c r="B176" s="5"/>
       <c r="C176" s="7"/>
@@ -2823,7 +2466,7 @@
       <c r="I176" s="1"/>
       <c r="J176" s="1"/>
     </row>
-    <row r="177">
+    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1"/>
       <c r="B177" s="5"/>
       <c r="C177" s="7"/>
@@ -2835,7 +2478,7 @@
       <c r="I177" s="1"/>
       <c r="J177" s="1"/>
     </row>
-    <row r="178">
+    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1"/>
       <c r="B178" s="5"/>
       <c r="C178" s="7"/>
@@ -2847,7 +2490,7 @@
       <c r="I178" s="1"/>
       <c r="J178" s="1"/>
     </row>
-    <row r="179">
+    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1"/>
       <c r="B179" s="5"/>
       <c r="C179" s="7"/>
@@ -2859,7 +2502,7 @@
       <c r="I179" s="1"/>
       <c r="J179" s="1"/>
     </row>
-    <row r="180">
+    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1"/>
       <c r="B180" s="5"/>
       <c r="C180" s="7"/>
@@ -2871,7 +2514,7 @@
       <c r="I180" s="1"/>
       <c r="J180" s="1"/>
     </row>
-    <row r="181">
+    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1"/>
       <c r="B181" s="5"/>
       <c r="C181" s="7"/>
@@ -2883,7 +2526,7 @@
       <c r="I181" s="1"/>
       <c r="J181" s="1"/>
     </row>
-    <row r="182">
+    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1"/>
       <c r="B182" s="5"/>
       <c r="C182" s="7"/>
@@ -2895,7 +2538,7 @@
       <c r="I182" s="1"/>
       <c r="J182" s="1"/>
     </row>
-    <row r="183">
+    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1"/>
       <c r="B183" s="5"/>
       <c r="C183" s="7"/>
@@ -2907,7 +2550,7 @@
       <c r="I183" s="1"/>
       <c r="J183" s="1"/>
     </row>
-    <row r="184">
+    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1"/>
       <c r="B184" s="5"/>
       <c r="C184" s="7"/>
@@ -2919,7 +2562,7 @@
       <c r="I184" s="1"/>
       <c r="J184" s="1"/>
     </row>
-    <row r="185">
+    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1"/>
       <c r="B185" s="5"/>
       <c r="C185" s="7"/>
@@ -2931,7 +2574,7 @@
       <c r="I185" s="1"/>
       <c r="J185" s="1"/>
     </row>
-    <row r="186">
+    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1"/>
       <c r="B186" s="5"/>
       <c r="C186" s="7"/>
@@ -2943,7 +2586,7 @@
       <c r="I186" s="1"/>
       <c r="J186" s="1"/>
     </row>
-    <row r="187">
+    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1"/>
       <c r="B187" s="5"/>
       <c r="C187" s="7"/>
@@ -2955,7 +2598,7 @@
       <c r="I187" s="1"/>
       <c r="J187" s="1"/>
     </row>
-    <row r="188">
+    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1"/>
       <c r="B188" s="5"/>
       <c r="C188" s="7"/>
@@ -2967,7 +2610,7 @@
       <c r="I188" s="1"/>
       <c r="J188" s="1"/>
     </row>
-    <row r="189">
+    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1"/>
       <c r="B189" s="5"/>
       <c r="C189" s="7"/>
@@ -2979,33 +2622,37 @@
       <c r="I189" s="1"/>
       <c r="J189" s="1"/>
     </row>
-    <row r="190">
+    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="3"/>
       <c r="F190" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$999"/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <autoFilter ref="A1:J999"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3037,28 +2684,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5">
-        <v>43974.790856481479</v>
-      </c>
-      <c r="C2" s="8">
-        <v>457.49000000000001</v>
-      </c>
-      <c r="D2" s="9">
-        <f>F2-E2</f>
-        <v>31.969999999999999</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="B2" s="5" t="n">
+        <v>43974.7908564815</v>
+      </c>
+      <c r="C2" s="8" t="n">
+        <v>457.49</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <f aca="false">F2-E2</f>
+        <v>31.97</v>
+      </c>
+      <c r="E2" s="3" t="n">
         <v>0.02</v>
       </c>
-      <c r="F2" s="3">
-        <v>31.989999999999998</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.069932019999999998</v>
+      <c r="F2" s="3" t="n">
+        <v>31.99</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>0.06993202</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -3067,438 +2714,438 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="9"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="9"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="9"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="9"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="9"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="9"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="9"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="9"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="4"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="9"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="9"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="9"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="4"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="4"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="9"/>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="4"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="9"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="4"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="9"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="4"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="9"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="4"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="9"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="4"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="9"/>
+      <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="4"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="9"/>
+      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="4"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="9"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="4"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="9"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="4"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="9"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="4"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="9"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="4"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="9"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="4"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="9"/>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="4"/>
@@ -3506,28 +3153,32 @@
       <c r="I45" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$J$995"/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <autoFilter ref="A1:J995"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M50" activeCellId="0" sqref="M50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3550,25 +3201,28 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="5">
-        <v>44011.182615740741</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.040000000000000001</v>
-      </c>
-      <c r="D2" s="9">
-        <f>C2/(1-E2)</f>
-        <v>0.047058823530000002</v>
-      </c>
-      <c r="E2" s="10">
-        <v>0.14999999999999999</v>
+      <c r="B2" s="5" t="n">
+        <v>44011.1826157407</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <f aca="false">C2/(1-E2)</f>
+        <v>0.04705882353</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>0.15</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -3576,410 +3230,464 @@
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4">
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>44041.1826157407</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <f aca="false">C3/(1-E3)</f>
+        <v>13.5363790186125</v>
+      </c>
+      <c r="E3" s="9" t="n">
+        <v>0.26125</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5">
+      <c r="H4" s="1"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="9"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6">
+      <c r="H5" s="1"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7">
+      <c r="H6" s="1"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8">
+      <c r="H7" s="1"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9">
+      <c r="H8" s="1"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10">
+      <c r="H9" s="1"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11">
+      <c r="H10" s="1"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12">
+      <c r="H11" s="1"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="5"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13">
+      <c r="H12" s="1"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14">
+      <c r="H13" s="1"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15">
+      <c r="H14" s="1"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16">
+      <c r="H15" s="1"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17">
+      <c r="H16" s="1"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18">
+      <c r="H17" s="1"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19">
+      <c r="H18" s="1"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="20">
+      <c r="H19" s="1"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21">
+      <c r="H20" s="1"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22">
+      <c r="H21" s="1"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23">
+      <c r="H22" s="1"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24">
+      <c r="H23" s="1"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="11"/>
-    </row>
-    <row r="25">
+      <c r="H24" s="1"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26">
+      <c r="H25" s="1"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27">
+      <c r="H26" s="1"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="5"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="12"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28">
+      <c r="H27" s="1"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29">
+      <c r="H28" s="1"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30">
+      <c r="H29" s="1"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31">
+      <c r="H30" s="1"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32">
+      <c r="H31" s="1"/>
+      <c r="I31" s="10"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33">
+      <c r="H32" s="1"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="5"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="12"/>
-    </row>
-    <row r="34">
+      <c r="D33" s="3"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="5"/>
       <c r="C34" s="3"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35">
+      <c r="D34" s="3"/>
+      <c r="E34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="5"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="12"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36">
+      <c r="D35" s="3"/>
+      <c r="E35" s="11"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="5"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="12"/>
-      <c r="J36" s="13"/>
-    </row>
-    <row r="37">
+      <c r="D36" s="3"/>
+      <c r="E36" s="11"/>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38">
+      <c r="D37" s="3"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="5"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39">
+      <c r="D38" s="3"/>
+      <c r="E38" s="11"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="5"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40">
+      <c r="D39" s="3"/>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="5"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="12"/>
-    </row>
-    <row r="41">
+      <c r="D40" s="3"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="5"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42">
+      <c r="D41" s="3"/>
+      <c r="E41" s="11"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="5"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="12"/>
-    </row>
-    <row r="43">
+      <c r="D42" s="3"/>
+      <c r="E42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="5"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44">
+      <c r="D43" s="3"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45">
+      <c r="D44" s="3"/>
+      <c r="E44" s="11"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="5"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="12"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$H$995"/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <autoFilter ref="A1:I995"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3987,7 +3695,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -3996,11 +3704,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="5">
-        <v>43951.964490740742</v>
-      </c>
-      <c r="B2" s="14">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>43951.9644907407</v>
+      </c>
+      <c r="B2" s="13" t="n">
         <v>0.01</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -4010,15 +3718,15 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5">
-        <v>43982.987303240741</v>
-      </c>
-      <c r="B3" s="14">
-        <v>0.029999999999999999</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>43982.9873032407</v>
+      </c>
+      <c r="B3" s="13" t="n">
+        <v>0.03</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -4027,15 +3735,15 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5">
-        <v>44012.983599537038</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0.040000000000000001</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>44012.983599537</v>
+      </c>
+      <c r="B4" s="13" t="n">
+        <v>0.04</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -4044,15 +3752,15 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5">
-        <v>44043.971724537034</v>
-      </c>
-      <c r="B5" s="14">
-        <v>0.050000000000000003</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>44043.971724537</v>
+      </c>
+      <c r="B5" s="13" t="n">
+        <v>0.05</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -4061,15 +3769,15 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5">
-        <v>44074.980624999997</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0.050000000000000003</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>44074.980625</v>
+      </c>
+      <c r="B6" s="13" t="n">
+        <v>0.05</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -4078,15 +3786,15 @@
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="5">
-        <v>44104.98642361111</v>
-      </c>
-      <c r="B7" s="14">
-        <v>0.059999999999999998</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>44104.9864236111</v>
+      </c>
+      <c r="B7" s="13" t="n">
+        <v>0.06</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -4095,15 +3803,15 @@
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5">
-        <v>44135.978865740741</v>
-      </c>
-      <c r="B8" s="14">
-        <v>0.059999999999999998</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>44135.9788657407</v>
+      </c>
+      <c r="B8" s="13" t="n">
+        <v>0.06</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
@@ -4112,144 +3820,148 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="14"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
-      <c r="B24" s="15"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$1000"/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <autoFilter ref="A1:E1000"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4257,7 +3969,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -4266,493 +3978,493 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="5">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
         <v>43871</v>
       </c>
-      <c r="B2" s="7">
-        <v>555.87779999999998</v>
+      <c r="B2" s="7" t="n">
+        <v>555.8778</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5"/>
       <c r="B3" s="7"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="7"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="7"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="7"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="7"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="7"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="7"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="7"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="7"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="7"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="7"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="7"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="7"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="7"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="7"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="7"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="7"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="7"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="7"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="7"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="7"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="7"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="7"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="7"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="7"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="7"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="7"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="7"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="7"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="7"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="7"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="7"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="7"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="7"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="7"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
       <c r="B44" s="7"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
       <c r="B45" s="7"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
       <c r="B46" s="7"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
       <c r="B47" s="7"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
       <c r="B48" s="7"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
       <c r="B49" s="7"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
       <c r="B50" s="7"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
       <c r="B51" s="7"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="7"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="7"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
       <c r="B54" s="7"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55">
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5"/>
       <c r="B55" s="7"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5"/>
       <c r="B56" s="7"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57">
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5"/>
       <c r="B57" s="7"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58">
+    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5"/>
       <c r="B58" s="7"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59">
+    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5"/>
       <c r="B59" s="7"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60">
+    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5"/>
       <c r="B60" s="7"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61">
+    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5"/>
       <c r="B61" s="7"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62">
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="5"/>
       <c r="B62" s="7"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63">
+    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5"/>
       <c r="B63" s="7"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64">
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5"/>
       <c r="B64" s="7"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65">
+    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5"/>
       <c r="B65" s="7"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66">
+    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
       <c r="B66" s="7"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67">
+    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5"/>
       <c r="B67" s="7"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68">
+    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5"/>
       <c r="B68" s="7"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69">
+    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5"/>
       <c r="B69" s="7"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70">
+    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5"/>
       <c r="B70" s="7"/>
       <c r="C70" s="1"/>
@@ -4760,10 +4472,14 @@
       <c r="E70" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$1000"/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <autoFilter ref="A1:E1000"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.700694444444444" right="0.700694444444444" top="0.752083333333333" bottom="0.752083333333333" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>